<commit_message>
Introduce time error, plotting improvements
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasnickel/Developer/Python/Henschke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD73BBBC-6230-9247-8FB2-DD053D12C6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647A3E6-015B-9B40-A5FF-80CB69DAECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Timestamp</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>t_E</t>
+  </si>
+  <si>
+    <t>ρ</t>
   </si>
 </sst>
 </file>
@@ -103,11 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -243,7 +247,7 @@
             <c:numRef>
               <c:f>Data!$C$2:$C$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -382,7 +386,7 @@
             <c:numRef>
               <c:f>Data!$D$2:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
@@ -397,7 +401,7 @@
                   <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.05</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.1</c:v>
@@ -549,7 +553,6 @@
         <c:axId val="22879792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -613,7 +616,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1301,7 +1304,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E1E6EB78-93AC-4049-947C-0A52AA2596CA}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="160" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1312,7 +1315,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307286" cy="6059714"/>
+    <xdr:ext cx="9318625" cy="6080125"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1">
@@ -1641,15 +1644,14 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="E2:G14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1675,10 +1677,10 @@
         <f>(A2-A$2)*86400</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>0.01</v>
       </c>
     </row>
@@ -1690,10 +1692,10 @@
         <f t="shared" ref="B3:B14" si="0">(A3-A$2)*86400</f>
         <v>37.999999999999993</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0.85</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -1705,10 +1707,10 @@
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0.77500000000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -1720,10 +1722,10 @@
         <f t="shared" si="0"/>
         <v>107.00000000000003</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>0.64</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -1735,11 +1737,11 @@
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D6">
-        <v>0.05</v>
+      <c r="D6" s="4">
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1750,10 +1752,10 @@
         <f t="shared" si="0"/>
         <v>308.99999999999994</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>0.51500000000000001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>0.1</v>
       </c>
     </row>
@@ -1765,10 +1767,10 @@
         <f t="shared" si="0"/>
         <v>376.99999999999994</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>0.49</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>0.17499999999999999</v>
       </c>
     </row>
@@ -1780,10 +1782,10 @@
         <f t="shared" si="0"/>
         <v>412</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>0.47499999999999998</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>0.19</v>
       </c>
     </row>
@@ -1795,10 +1797,10 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>0.44</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -1810,10 +1812,10 @@
         <f t="shared" si="0"/>
         <v>631.00000000000011</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>0.41</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>0.32500000000000001</v>
       </c>
     </row>
@@ -1825,10 +1827,10 @@
         <f t="shared" si="0"/>
         <v>775.00000000000011</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>0.39500000000000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>0.35</v>
       </c>
     </row>
@@ -1840,10 +1842,10 @@
         <f t="shared" si="0"/>
         <v>1035.9999999999998</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>0.38</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>0.36</v>
       </c>
     </row>
@@ -1855,10 +1857,10 @@
         <f t="shared" si="0"/>
         <v>1586.9999999999998</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>0.375</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>0.36499999999999999</v>
       </c>
     </row>
@@ -1869,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C8D33A-7D60-41F1-8E76-471890D6F029}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1880,7 +1882,7 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1891,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1911,6 +1913,21 @@
       </c>
       <c r="C3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>918.8</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <f>C4-B4</f>
+        <v>81.200000000000045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix settler.py, centralize methods
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasnickel/Developer/Python/Henschke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F741A23F-1D2B-7040-9421-4D4D98CCBE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B4B74C-F9EF-8D48-A180-BCAEFCDD77AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" activeTab="1" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Timestamp</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Pas</t>
+  </si>
+  <si>
+    <t>η_v</t>
   </si>
 </sst>
 </file>
@@ -1898,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C8D33A-7D60-41F1-8E76-471890D6F029}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1912,7 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -1934,8 +1937,11 @@
       <c r="I1" t="s">
         <v>17</v>
       </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1963,8 +1969,11 @@
       <c r="I2">
         <v>4.9140000000000003E-2</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1987,6 +1996,9 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>